<commit_message>
Add NLP exam time to the DCS timetable.
</commit_message>
<xml_diff>
--- a/dcs_timetable.xlsx
+++ b/dcs_timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arghasarkar/Documents/UniversityWork/masters/exam_paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArghaWin10\Documents\WarwickMasters\exam-papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEABD49A-9E6D-C145-9B13-694D1F39E7C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90084D17-9356-4DE8-8AB0-C60C89DB9929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="460" windowWidth="27640" windowHeight="16540" xr2:uid="{93AE4905-63E8-2B46-90A6-AD30EDC67393}"/>
+    <workbookView xWindow="7545" yWindow="1215" windowWidth="28800" windowHeight="11385" xr2:uid="{93AE4905-63E8-2B46-90A6-AD30EDC67393}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Computer Science</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Module name</t>
+  </si>
+  <si>
+    <t>CS9180</t>
+  </si>
+  <si>
+    <t>Natural Language Processing</t>
   </si>
 </sst>
 </file>
@@ -144,12 +150,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -164,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -173,6 +185,13 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,18 +509,18 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.375" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>25</v>
       </c>
@@ -518,75 +537,75 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1">
-        <v>43615</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5">
+        <v>43598</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.39583333333333298</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
-        <v>43598</v>
+        <v>43599</v>
       </c>
       <c r="E3" s="2">
         <v>0.39583333333333298</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>43607</v>
+        <v>43600</v>
       </c>
       <c r="E4" s="2">
         <v>0.39583333333333298</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43624</v>
-      </c>
-      <c r="E5" s="2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="5">
+        <v>43601</v>
+      </c>
+      <c r="E5" s="6">
         <v>0.39583333333333298</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -603,206 +622,222 @@
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1">
-        <v>43599</v>
-      </c>
-      <c r="E7" s="2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="5">
+        <v>43607</v>
+      </c>
+      <c r="E7" s="6">
         <v>0.39583333333333298</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43608</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D9" s="1">
         <v>43613</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43616</v>
       </c>
       <c r="E9" s="2">
         <v>0.39583333333333298</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="5">
+        <v>43615</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="5">
+        <v>43616</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.39583333333333298</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D12" s="5">
         <v>43617</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E12" s="6">
         <v>0.39583333333333298</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43600</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.39583333333333298</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D13" s="1">
         <v>43621</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>43608</v>
       </c>
       <c r="E13" s="2">
         <v>0.58333333333333304</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>43624</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.39583333333333298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D27" s="1"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D28" s="1"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D30" s="1"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D44" s="1"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D46" s="1"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
+    <sortCondition ref="D14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add venues to exam timetable.
</commit_message>
<xml_diff>
--- a/dcs_timetable.xlsx
+++ b/dcs_timetable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ArghaWin10\Documents\WarwickMasters\exam-papers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arghasarkar/Documents/UniversityWork/masters/exam_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90084D17-9356-4DE8-8AB0-C60C89DB9929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BDE9D1E-6289-A843-A02B-EA56CEADB899}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7545" yWindow="1215" windowWidth="28800" windowHeight="11385" xr2:uid="{93AE4905-63E8-2B46-90A6-AD30EDC67393}"/>
+    <workbookView xWindow="0" yWindow="1220" windowWidth="28800" windowHeight="16780" xr2:uid="{93AE4905-63E8-2B46-90A6-AD30EDC67393}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Computer Science</t>
   </si>
@@ -127,6 +127,27 @@
   </si>
   <si>
     <t>Natural Language Processing</t>
+  </si>
+  <si>
+    <t>Main Hall, Old Sports Centre</t>
+  </si>
+  <si>
+    <t>Desso Hall, Old Sports Centre</t>
+  </si>
+  <si>
+    <t>Westwood Games Hall</t>
+  </si>
+  <si>
+    <t>Rootes Restaurant Area</t>
+  </si>
+  <si>
+    <t>Panorama Room, Rootes Building</t>
+  </si>
+  <si>
+    <t>OC1.09, Oculus Building</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
@@ -164,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -172,11 +193,275 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -184,13 +469,84 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -506,90 +862,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DABF4097-FCFD-4E42-8E73-63E7B44CC535}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="17">
         <v>43598</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="18">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="26"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="7">
         <v>43599</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="8">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="7">
         <v>43600</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="8">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="F4" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -604,26 +980,36 @@
       <c r="E5" s="6">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" s="32"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="7">
         <v>43602</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="8">
         <v>0.58333333333333304</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="F6" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -638,43 +1024,58 @@
       <c r="E7" s="6">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="31"/>
+      <c r="H7" s="32"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="7">
         <v>43608</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="8">
         <v>0.58333333333333304</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="7">
         <v>43613</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="8">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="F9" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -689,9 +1090,14 @@
       <c r="E10" s="6">
         <v>0.58333333333333304</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F10" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -706,9 +1112,14 @@
       <c r="E11" s="6">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="F11" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -723,121 +1134,92 @@
       <c r="E12" s="6">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="31"/>
+      <c r="H12" s="32"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="7">
         <v>43621</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="8">
         <v>0.58333333333333304</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F13" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="13">
         <v>43624</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="14">
         <v>0.39583333333333298</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="1"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="1"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="1"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="1"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="1"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="1"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D30" s="1"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D44" s="1"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D46" s="1"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" s="1"/>
       <c r="E49" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
-    <sortCondition ref="D14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F14">
+    <sortCondition ref="D2"/>
   </sortState>
+  <mergeCells count="14">
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>